<commit_message>
updating habitat extent, condition, and trend data. waiting on NOAA coral reef indicators and beach indicators from DLNR
</commit_message>
<xml_diff>
--- a/prep/HAB/hab_beaches_romine.xlsx
+++ b/prep/HAB/hab_beaches_romine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1230" windowWidth="26835" windowHeight="11190"/>
+    <workbookView xWindow="-4815" yWindow="2115" windowWidth="26835" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>rgn_id</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>health(percent not erroding)</t>
+  </si>
+  <si>
+    <t>short_percent_change_km_yr</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,11 +413,11 @@
     <col min="8" max="8" width="21.140625" customWidth="1"/>
     <col min="9" max="10" width="15.85546875" customWidth="1"/>
     <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="31.5703125" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" customWidth="1"/>
+    <col min="12" max="13" width="31.5703125" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,10 +455,13 @@
         <v>1</v>
       </c>
       <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -494,11 +500,15 @@
         <v>-6.0000000000000005E-2</v>
       </c>
       <c r="M2">
+        <f>L2/1000</f>
+        <v>-6.0000000000000002E-5</v>
+      </c>
+      <c r="N2">
         <f>K2*0.001</f>
         <v>-1.1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -538,11 +548,15 @@
         <v>-0.15</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M5" si="2">K3*0.001</f>
+        <f t="shared" ref="M3:M5" si="2">L3/1000</f>
+        <v>-1.4999999999999999E-4</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N5" si="3">K3*0.001</f>
         <v>-1.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -583,10 +597,14 @@
       </c>
       <c r="M4">
         <f t="shared" si="2"/>
+        <v>-5.0000000000000002E-5</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="3"/>
         <v>-6.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -627,6 +645,10 @@
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
         <v>-1.1E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjusted beach trend data to annual % loss of beaches instead pf long term errosional rate
</commit_message>
<xml_diff>
--- a/prep/HAB/hab_beaches_romine.xlsx
+++ b/prep/HAB/hab_beaches_romine.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eschemmel/Documents/github/mhi/prep/HAB/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4815" yWindow="2115" windowWidth="26835" windowHeight="11190"/>
+    <workbookView xWindow="0" yWindow="2120" windowWidth="26840" windowHeight="11200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>rgn_id</t>
   </si>
@@ -61,12 +66,18 @@
   </si>
   <si>
     <t>short_percent_change_km_yr</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>trend in % beach lost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,6 +118,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -155,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +202,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,6 +254,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -398,26 +446,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="13" width="31.5703125" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="10" width="21.1640625" customWidth="1"/>
+    <col min="11" max="12" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="30.6640625" customWidth="1"/>
+    <col min="14" max="15" width="31.5" customWidth="1"/>
+    <col min="16" max="16" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,25 +491,31 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -488,27 +542,34 @@
       <c r="H2">
         <v>9</v>
       </c>
+      <c r="I2">
+        <v>80</v>
+      </c>
       <c r="J2">
-        <f>AVERAGE(J3:J5)</f>
-        <v>7.166666666666667</v>
-      </c>
-      <c r="K2">
-        <v>-0.11</v>
+        <f>-(H2/100)/I2</f>
+        <v>-1.1249999999999999E-3</v>
       </c>
       <c r="L2">
         <f>AVERAGE(L3:L5)</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="M2">
+        <v>-0.11</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(N3:N5)</f>
         <v>-6.0000000000000005E-2</v>
       </c>
-      <c r="M2">
-        <f>L2/1000</f>
+      <c r="O2">
+        <f>N2/1000</f>
         <v>-6.0000000000000002E-5</v>
       </c>
-      <c r="N2">
-        <f>K2*0.001</f>
+      <c r="P2">
+        <f>M2*0.001</f>
         <v>-1.1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -535,28 +596,35 @@
       <c r="H3">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>80</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="2">-(H3/100)/I3</f>
+        <v>-1.3749999999999999E-3</v>
+      </c>
+      <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>6.8</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>-0.17</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>-0.15</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M5" si="2">L3/1000</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O5" si="3">N3/1000</f>
         <v>-1.4999999999999999E-4</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N5" si="3">K3*0.001</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="4">M3*0.001</f>
         <v>-1.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -584,27 +652,34 @@
         <v>8</v>
       </c>
       <c r="I4">
+        <v>80</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>-1E-3</v>
+      </c>
+      <c r="K4">
         <v>107</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>8.6999999999999993</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>-0.06</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>-0.05</v>
       </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
+      <c r="O4">
+        <f t="shared" si="3"/>
         <v>-5.0000000000000002E-5</v>
       </c>
-      <c r="N4">
-        <f t="shared" si="3"/>
+      <c r="P4">
+        <f t="shared" si="4"/>
         <v>-6.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -632,23 +707,30 @@
         <v>8</v>
       </c>
       <c r="I5">
+        <v>80</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>-1E-3</v>
+      </c>
+      <c r="K5">
         <v>75</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>6</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>-0.11</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>0.02</v>
       </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
+      <c r="O5">
+        <f t="shared" si="3"/>
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="N5">
-        <f t="shared" si="3"/>
+      <c r="P5">
+        <f t="shared" si="4"/>
         <v>-1.1E-4</v>
       </c>
     </row>
@@ -658,24 +740,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>